<commit_message>
Añadidos test de ejercicio C05
</commit_message>
<xml_diff>
--- a/docs/sdi2021-entrega2-1005.xlsx
+++ b/docs/sdi2021-entrega2-1005.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Uniovi\Asignaturas\SDI\SDI_I4\Practicas\Practica Node\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DAC852-FCA4-48B0-9590-3D63917116D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D532F14E-9C70-4A1E-B350-FF00DA3F487A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="119">
   <si>
     <t>Puntuación (Para rellenar por el profesor)</t>
   </si>
@@ -468,6 +468,9 @@
   </si>
   <si>
     <t>S7</t>
+  </si>
+  <si>
+    <t>Se ha tenido que meter una carga de otra página de por medio para que le de tiempo a la peticion post a tener una respuesta</t>
   </si>
 </sst>
 </file>
@@ -1026,8 +1029,82 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1051,82 +1128,8 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1410,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E127" sqref="E127"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1448,7 +1451,7 @@
     <row r="4" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="72">
         <f>H40</f>
-        <v>5.5</v>
+        <v>6.3000000000000007</v>
       </c>
       <c r="C4" s="72"/>
       <c r="D4" s="72"/>
@@ -1494,7 +1497,7 @@
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B8" s="75">
         <f>B4-B6</f>
-        <v>5.5</v>
+        <v>6.3000000000000007</v>
       </c>
       <c r="C8" s="75"/>
       <c r="D8" s="75"/>
@@ -2254,7 +2257,7 @@
       </c>
       <c r="E35" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="31">
         <f t="shared" si="2"/>
@@ -2262,11 +2265,11 @@
       </c>
       <c r="G35" s="31">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="31">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -2285,7 +2288,7 @@
       </c>
       <c r="E36" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F36" s="31">
         <f t="shared" si="2"/>
@@ -2293,11 +2296,11 @@
       </c>
       <c r="G36" s="31">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H36" s="31">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
@@ -2408,7 +2411,7 @@
       </c>
       <c r="H40" s="11">
         <f>SUM(H13:H39)</f>
-        <v>5.5</v>
+        <v>6.3000000000000007</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>13</v>
@@ -2454,13 +2457,13 @@
       <c r="B43" s="52">
         <v>1</v>
       </c>
-      <c r="C43" s="60" t="s">
+      <c r="C43" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="85"/>
       <c r="H43" s="36"/>
       <c r="I43" s="37"/>
       <c r="J43" s="38"/>
@@ -2473,13 +2476,13 @@
       <c r="B44" s="53">
         <v>2</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="C44" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="61"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
+      <c r="D44" s="85"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="85"/>
       <c r="H44" s="36"/>
       <c r="I44" s="37"/>
       <c r="J44" s="38"/>
@@ -2492,13 +2495,13 @@
       <c r="B45" s="53">
         <v>3</v>
       </c>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
+      <c r="D45" s="85"/>
+      <c r="E45" s="85"/>
+      <c r="F45" s="85"/>
+      <c r="G45" s="85"/>
       <c r="H45" s="36"/>
       <c r="I45" s="37"/>
       <c r="J45" s="38"/>
@@ -2511,11 +2514,11 @@
       <c r="B46" s="53">
         <v>4</v>
       </c>
-      <c r="C46" s="60"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
+      <c r="C46" s="84"/>
+      <c r="D46" s="85"/>
+      <c r="E46" s="85"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="85"/>
       <c r="H46" s="36"/>
       <c r="I46" s="37"/>
       <c r="J46" s="38"/>
@@ -2528,11 +2531,11 @@
       <c r="B47" s="53">
         <v>5</v>
       </c>
-      <c r="C47" s="62"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="61"/>
-      <c r="G47" s="61"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="85"/>
+      <c r="E47" s="85"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="85"/>
       <c r="H47" s="36"/>
       <c r="I47" s="37"/>
       <c r="J47" s="38"/>
@@ -2545,11 +2548,11 @@
       <c r="B48" s="53">
         <v>6</v>
       </c>
-      <c r="C48" s="62"/>
-      <c r="D48" s="61"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="61"/>
-      <c r="G48" s="61"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="85"/>
+      <c r="E48" s="85"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="85"/>
       <c r="H48" s="36"/>
       <c r="I48" s="37"/>
       <c r="J48" s="38"/>
@@ -2562,11 +2565,11 @@
       <c r="B49" s="53">
         <v>7</v>
       </c>
-      <c r="C49" s="62"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="85"/>
+      <c r="E49" s="85"/>
+      <c r="F49" s="85"/>
+      <c r="G49" s="85"/>
       <c r="H49" s="36"/>
       <c r="I49" s="37"/>
       <c r="J49" s="38"/>
@@ -2579,11 +2582,11 @@
       <c r="B50" s="53">
         <v>8</v>
       </c>
-      <c r="C50" s="62"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="85"/>
+      <c r="F50" s="85"/>
+      <c r="G50" s="85"/>
       <c r="H50" s="36"/>
       <c r="I50" s="40"/>
       <c r="J50" s="38"/>
@@ -2596,11 +2599,11 @@
       <c r="B51" s="53">
         <v>9</v>
       </c>
-      <c r="C51" s="62"/>
-      <c r="D51" s="61"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="85"/>
+      <c r="E51" s="85"/>
+      <c r="F51" s="85"/>
+      <c r="G51" s="85"/>
       <c r="H51" s="36"/>
       <c r="I51" s="37"/>
       <c r="J51" s="38"/>
@@ -2613,11 +2616,11 @@
       <c r="B52" s="53">
         <v>10</v>
       </c>
-      <c r="C52" s="62"/>
-      <c r="D52" s="61"/>
-      <c r="E52" s="61"/>
-      <c r="F52" s="61"/>
-      <c r="G52" s="61"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="85"/>
+      <c r="E52" s="85"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="85"/>
       <c r="H52" s="36"/>
       <c r="I52" s="37"/>
       <c r="J52" s="38"/>
@@ -2630,11 +2633,11 @@
       <c r="B53" s="53">
         <v>11</v>
       </c>
-      <c r="C53" s="62"/>
-      <c r="D53" s="61"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="85"/>
       <c r="H53" s="36"/>
       <c r="I53" s="37"/>
       <c r="J53" s="38"/>
@@ -2647,11 +2650,11 @@
       <c r="B54" s="53">
         <v>12</v>
       </c>
-      <c r="C54" s="62"/>
-      <c r="D54" s="61"/>
-      <c r="E54" s="61"/>
-      <c r="F54" s="61"/>
-      <c r="G54" s="61"/>
+      <c r="C54" s="86"/>
+      <c r="D54" s="85"/>
+      <c r="E54" s="85"/>
+      <c r="F54" s="85"/>
+      <c r="G54" s="85"/>
       <c r="H54" s="36"/>
       <c r="I54" s="37"/>
       <c r="J54" s="38"/>
@@ -2664,11 +2667,11 @@
       <c r="B55" s="53">
         <v>13</v>
       </c>
-      <c r="C55" s="62"/>
-      <c r="D55" s="61"/>
-      <c r="E55" s="61"/>
-      <c r="F55" s="61"/>
-      <c r="G55" s="61"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="85"/>
+      <c r="E55" s="85"/>
+      <c r="F55" s="85"/>
+      <c r="G55" s="85"/>
       <c r="H55" s="36"/>
       <c r="I55" s="37"/>
       <c r="J55" s="38"/>
@@ -2681,11 +2684,11 @@
       <c r="B56" s="53">
         <v>14</v>
       </c>
-      <c r="C56" s="62"/>
-      <c r="D56" s="61"/>
-      <c r="E56" s="61"/>
-      <c r="F56" s="61"/>
-      <c r="G56" s="61"/>
+      <c r="C56" s="86"/>
+      <c r="D56" s="85"/>
+      <c r="E56" s="85"/>
+      <c r="F56" s="85"/>
+      <c r="G56" s="85"/>
       <c r="H56" s="36"/>
       <c r="I56" s="37"/>
       <c r="J56" s="38"/>
@@ -2698,11 +2701,11 @@
       <c r="B57" s="53">
         <v>15</v>
       </c>
-      <c r="C57" s="62"/>
-      <c r="D57" s="61"/>
-      <c r="E57" s="61"/>
-      <c r="F57" s="61"/>
-      <c r="G57" s="61"/>
+      <c r="C57" s="86"/>
+      <c r="D57" s="85"/>
+      <c r="E57" s="85"/>
+      <c r="F57" s="85"/>
+      <c r="G57" s="85"/>
       <c r="H57" s="36"/>
       <c r="I57" s="37"/>
       <c r="J57" s="38"/>
@@ -2715,11 +2718,11 @@
       <c r="B58" s="53">
         <v>16</v>
       </c>
-      <c r="C58" s="62"/>
-      <c r="D58" s="61"/>
-      <c r="E58" s="61"/>
-      <c r="F58" s="61"/>
-      <c r="G58" s="61"/>
+      <c r="C58" s="86"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="85"/>
+      <c r="F58" s="85"/>
+      <c r="G58" s="85"/>
       <c r="H58" s="36"/>
       <c r="I58" s="37"/>
       <c r="J58" s="38"/>
@@ -2732,11 +2735,11 @@
       <c r="B59" s="53">
         <v>17</v>
       </c>
-      <c r="C59" s="62"/>
-      <c r="D59" s="61"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="61"/>
-      <c r="G59" s="61"/>
+      <c r="C59" s="86"/>
+      <c r="D59" s="85"/>
+      <c r="E59" s="85"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
       <c r="H59" s="36"/>
       <c r="I59" s="37"/>
       <c r="J59" s="38"/>
@@ -2749,11 +2752,11 @@
       <c r="B60" s="53">
         <v>18</v>
       </c>
-      <c r="C60" s="62"/>
-      <c r="D60" s="61"/>
-      <c r="E60" s="61"/>
-      <c r="F60" s="61"/>
-      <c r="G60" s="61"/>
+      <c r="C60" s="86"/>
+      <c r="D60" s="85"/>
+      <c r="E60" s="85"/>
+      <c r="F60" s="85"/>
+      <c r="G60" s="85"/>
       <c r="H60" s="36"/>
       <c r="I60" s="37"/>
       <c r="J60" s="38"/>
@@ -2766,11 +2769,11 @@
       <c r="B61" s="53">
         <v>19</v>
       </c>
-      <c r="C61" s="62"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="61"/>
+      <c r="C61" s="86"/>
+      <c r="D61" s="85"/>
+      <c r="E61" s="85"/>
+      <c r="F61" s="85"/>
+      <c r="G61" s="85"/>
       <c r="H61" s="36"/>
       <c r="I61" s="37"/>
       <c r="J61" s="38"/>
@@ -2783,11 +2786,11 @@
       <c r="B62" s="53">
         <v>20</v>
       </c>
-      <c r="C62" s="62"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="61"/>
-      <c r="G62" s="61"/>
+      <c r="C62" s="86"/>
+      <c r="D62" s="85"/>
+      <c r="E62" s="85"/>
+      <c r="F62" s="85"/>
+      <c r="G62" s="85"/>
       <c r="H62" s="36"/>
       <c r="I62" s="37"/>
       <c r="J62" s="38"/>
@@ -2800,11 +2803,11 @@
       <c r="B63" s="53">
         <v>21</v>
       </c>
-      <c r="C63" s="62"/>
-      <c r="D63" s="61"/>
-      <c r="E63" s="61"/>
-      <c r="F63" s="61"/>
-      <c r="G63" s="61"/>
+      <c r="C63" s="86"/>
+      <c r="D63" s="85"/>
+      <c r="E63" s="85"/>
+      <c r="F63" s="85"/>
+      <c r="G63" s="85"/>
       <c r="H63" s="36"/>
       <c r="I63" s="40"/>
       <c r="J63" s="38"/>
@@ -2817,11 +2820,11 @@
       <c r="B64" s="53">
         <v>22</v>
       </c>
-      <c r="C64" s="62"/>
-      <c r="D64" s="61"/>
-      <c r="E64" s="61"/>
-      <c r="F64" s="61"/>
-      <c r="G64" s="61"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="85"/>
+      <c r="E64" s="85"/>
+      <c r="F64" s="85"/>
+      <c r="G64" s="85"/>
       <c r="H64" s="36"/>
       <c r="I64" s="40"/>
       <c r="J64" s="38"/>
@@ -2834,11 +2837,11 @@
       <c r="B65" s="53">
         <v>23</v>
       </c>
-      <c r="C65" s="62"/>
-      <c r="D65" s="61"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="61"/>
-      <c r="G65" s="61"/>
+      <c r="C65" s="86"/>
+      <c r="D65" s="85"/>
+      <c r="E65" s="85"/>
+      <c r="F65" s="85"/>
+      <c r="G65" s="85"/>
       <c r="H65" s="36"/>
       <c r="I65" s="40"/>
       <c r="J65" s="38"/>
@@ -2851,11 +2854,11 @@
       <c r="B66" s="53">
         <v>24</v>
       </c>
-      <c r="C66" s="62"/>
-      <c r="D66" s="61"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="61"/>
-      <c r="G66" s="61"/>
+      <c r="C66" s="86"/>
+      <c r="D66" s="85"/>
+      <c r="E66" s="85"/>
+      <c r="F66" s="85"/>
+      <c r="G66" s="85"/>
       <c r="H66" s="36"/>
       <c r="I66" s="40"/>
       <c r="J66" s="38"/>
@@ -2868,11 +2871,11 @@
       <c r="B67" s="53">
         <v>25</v>
       </c>
-      <c r="C67" s="62"/>
-      <c r="D67" s="61"/>
-      <c r="E67" s="61"/>
-      <c r="F67" s="61"/>
-      <c r="G67" s="61"/>
+      <c r="C67" s="86"/>
+      <c r="D67" s="85"/>
+      <c r="E67" s="85"/>
+      <c r="F67" s="85"/>
+      <c r="G67" s="85"/>
       <c r="H67" s="36"/>
       <c r="I67" s="40"/>
       <c r="J67" s="38"/>
@@ -2885,11 +2888,11 @@
       <c r="B68" s="53">
         <v>26</v>
       </c>
-      <c r="C68" s="62"/>
-      <c r="D68" s="61"/>
-      <c r="E68" s="61"/>
-      <c r="F68" s="61"/>
-      <c r="G68" s="61"/>
+      <c r="C68" s="86"/>
+      <c r="D68" s="85"/>
+      <c r="E68" s="85"/>
+      <c r="F68" s="85"/>
+      <c r="G68" s="85"/>
       <c r="H68" s="36"/>
       <c r="I68" s="40"/>
       <c r="J68" s="38"/>
@@ -2902,11 +2905,11 @@
       <c r="B69" s="53">
         <v>27</v>
       </c>
-      <c r="C69" s="62"/>
-      <c r="D69" s="61"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="61"/>
-      <c r="G69" s="61"/>
+      <c r="C69" s="86"/>
+      <c r="D69" s="85"/>
+      <c r="E69" s="85"/>
+      <c r="F69" s="85"/>
+      <c r="G69" s="85"/>
       <c r="H69" s="36"/>
       <c r="I69" s="40"/>
       <c r="J69" s="38"/>
@@ -2919,11 +2922,11 @@
       <c r="B70" s="53">
         <v>28</v>
       </c>
-      <c r="C70" s="62"/>
-      <c r="D70" s="61"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="61"/>
-      <c r="G70" s="61"/>
+      <c r="C70" s="86"/>
+      <c r="D70" s="85"/>
+      <c r="E70" s="85"/>
+      <c r="F70" s="85"/>
+      <c r="G70" s="85"/>
       <c r="H70" s="36"/>
       <c r="I70" s="40"/>
       <c r="J70" s="38"/>
@@ -2936,11 +2939,11 @@
       <c r="B71" s="53">
         <v>29</v>
       </c>
-      <c r="C71" s="62"/>
-      <c r="D71" s="61"/>
-      <c r="E71" s="61"/>
-      <c r="F71" s="61"/>
-      <c r="G71" s="61"/>
+      <c r="C71" s="86"/>
+      <c r="D71" s="85"/>
+      <c r="E71" s="85"/>
+      <c r="F71" s="85"/>
+      <c r="G71" s="85"/>
       <c r="H71" s="36"/>
       <c r="I71" s="40"/>
       <c r="J71" s="38"/>
@@ -2953,11 +2956,11 @@
       <c r="B72" s="53">
         <v>30</v>
       </c>
-      <c r="C72" s="62"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
+      <c r="C72" s="86"/>
+      <c r="D72" s="85"/>
+      <c r="E72" s="85"/>
+      <c r="F72" s="85"/>
+      <c r="G72" s="85"/>
       <c r="H72" s="36"/>
       <c r="I72" s="40"/>
       <c r="J72" s="38"/>
@@ -2970,11 +2973,11 @@
       <c r="B73" s="53">
         <v>31</v>
       </c>
-      <c r="C73" s="62"/>
-      <c r="D73" s="64"/>
-      <c r="E73" s="64"/>
-      <c r="F73" s="64"/>
-      <c r="G73" s="64"/>
+      <c r="C73" s="86"/>
+      <c r="D73" s="88"/>
+      <c r="E73" s="88"/>
+      <c r="F73" s="88"/>
+      <c r="G73" s="88"/>
       <c r="H73" s="36"/>
       <c r="I73" s="37"/>
       <c r="J73" s="38"/>
@@ -2987,11 +2990,11 @@
       <c r="B74" s="53">
         <v>32</v>
       </c>
-      <c r="C74" s="62"/>
-      <c r="D74" s="64"/>
-      <c r="E74" s="64"/>
-      <c r="F74" s="64"/>
-      <c r="G74" s="64"/>
+      <c r="C74" s="86"/>
+      <c r="D74" s="88"/>
+      <c r="E74" s="88"/>
+      <c r="F74" s="88"/>
+      <c r="G74" s="88"/>
       <c r="H74" s="36"/>
       <c r="I74" s="37"/>
       <c r="J74" s="38"/>
@@ -3004,11 +3007,11 @@
       <c r="B75" s="53">
         <v>33</v>
       </c>
-      <c r="C75" s="62"/>
-      <c r="D75" s="64"/>
-      <c r="E75" s="64"/>
-      <c r="F75" s="64"/>
-      <c r="G75" s="64"/>
+      <c r="C75" s="86"/>
+      <c r="D75" s="88"/>
+      <c r="E75" s="88"/>
+      <c r="F75" s="88"/>
+      <c r="G75" s="88"/>
       <c r="H75" s="36"/>
       <c r="I75" s="37"/>
       <c r="J75" s="38"/>
@@ -3021,11 +3024,11 @@
       <c r="B76" s="54">
         <v>34</v>
       </c>
-      <c r="C76" s="65"/>
-      <c r="D76" s="66"/>
-      <c r="E76" s="66"/>
-      <c r="F76" s="66"/>
-      <c r="G76" s="66"/>
+      <c r="C76" s="89"/>
+      <c r="D76" s="90"/>
+      <c r="E76" s="90"/>
+      <c r="F76" s="90"/>
+      <c r="G76" s="90"/>
       <c r="H76" s="41"/>
       <c r="I76" s="37"/>
       <c r="J76" s="38"/>
@@ -3038,11 +3041,11 @@
       <c r="B77" s="55">
         <v>35</v>
       </c>
-      <c r="C77" s="63"/>
-      <c r="D77" s="63"/>
-      <c r="E77" s="63"/>
-      <c r="F77" s="63"/>
-      <c r="G77" s="63"/>
+      <c r="C77" s="87"/>
+      <c r="D77" s="87"/>
+      <c r="E77" s="87"/>
+      <c r="F77" s="87"/>
+      <c r="G77" s="87"/>
       <c r="H77" s="42"/>
       <c r="I77" s="37"/>
       <c r="J77" s="38"/>
@@ -3055,11 +3058,11 @@
       <c r="B78" s="55">
         <v>36</v>
       </c>
-      <c r="C78" s="63"/>
-      <c r="D78" s="63"/>
-      <c r="E78" s="63"/>
-      <c r="F78" s="63"/>
-      <c r="G78" s="63"/>
+      <c r="C78" s="87"/>
+      <c r="D78" s="87"/>
+      <c r="E78" s="87"/>
+      <c r="F78" s="87"/>
+      <c r="G78" s="87"/>
       <c r="H78" s="42"/>
       <c r="I78" s="37"/>
       <c r="J78" s="38"/>
@@ -3072,11 +3075,11 @@
       <c r="B79" s="55">
         <v>38</v>
       </c>
-      <c r="C79" s="63"/>
-      <c r="D79" s="63"/>
-      <c r="E79" s="63"/>
-      <c r="F79" s="63"/>
-      <c r="G79" s="63"/>
+      <c r="C79" s="87"/>
+      <c r="D79" s="87"/>
+      <c r="E79" s="87"/>
+      <c r="F79" s="87"/>
+      <c r="G79" s="87"/>
       <c r="H79" s="42"/>
       <c r="I79" s="43"/>
       <c r="J79" s="38"/>
@@ -3089,11 +3092,11 @@
       <c r="B80" s="55">
         <v>39</v>
       </c>
-      <c r="C80" s="63"/>
-      <c r="D80" s="63"/>
-      <c r="E80" s="63"/>
-      <c r="F80" s="63"/>
-      <c r="G80" s="63"/>
+      <c r="C80" s="87"/>
+      <c r="D80" s="87"/>
+      <c r="E80" s="87"/>
+      <c r="F80" s="87"/>
+      <c r="G80" s="87"/>
       <c r="H80" s="42"/>
       <c r="I80" s="43"/>
       <c r="J80" s="38"/>
@@ -3106,11 +3109,11 @@
       <c r="B81" s="55">
         <v>40</v>
       </c>
-      <c r="C81" s="63"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="63"/>
-      <c r="F81" s="63"/>
-      <c r="G81" s="63"/>
+      <c r="C81" s="87"/>
+      <c r="D81" s="87"/>
+      <c r="E81" s="87"/>
+      <c r="F81" s="87"/>
+      <c r="G81" s="87"/>
       <c r="H81" s="42"/>
       <c r="I81" s="43"/>
       <c r="J81" s="38"/>
@@ -3198,24 +3201,24 @@
       <c r="E87" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F87" s="84"/>
-      <c r="G87" s="85"/>
-      <c r="H87" s="85"/>
-      <c r="J87" s="59" t="s">
+      <c r="F87" s="63"/>
+      <c r="G87" s="64"/>
+      <c r="H87" s="64"/>
+      <c r="J87" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="K87" s="59"/>
-      <c r="L87" s="59"/>
-      <c r="M87" s="59"/>
-      <c r="N87" s="59"/>
-      <c r="O87" s="59"/>
-      <c r="P87" s="59"/>
-      <c r="Q87" s="59"/>
-      <c r="R87" s="59"/>
-      <c r="S87" s="59"/>
-      <c r="T87" s="59"/>
-      <c r="U87" s="59"/>
-      <c r="V87" s="59"/>
+      <c r="K87" s="91"/>
+      <c r="L87" s="91"/>
+      <c r="M87" s="91"/>
+      <c r="N87" s="91"/>
+      <c r="O87" s="91"/>
+      <c r="P87" s="91"/>
+      <c r="Q87" s="91"/>
+      <c r="R87" s="91"/>
+      <c r="S87" s="91"/>
+      <c r="T87" s="91"/>
+      <c r="U87" s="91"/>
+      <c r="V87" s="91"/>
     </row>
     <row r="88" spans="2:32" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="48">
@@ -3230,24 +3233,24 @@
       <c r="E88" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F88" s="84"/>
-      <c r="G88" s="85"/>
-      <c r="H88" s="85"/>
-      <c r="J88" s="59" t="s">
+      <c r="F88" s="63"/>
+      <c r="G88" s="64"/>
+      <c r="H88" s="64"/>
+      <c r="J88" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="K88" s="59"/>
-      <c r="L88" s="59"/>
-      <c r="M88" s="59"/>
-      <c r="N88" s="59"/>
-      <c r="O88" s="59"/>
-      <c r="P88" s="59"/>
-      <c r="Q88" s="59"/>
-      <c r="R88" s="59"/>
-      <c r="S88" s="59"/>
-      <c r="T88" s="59"/>
-      <c r="U88" s="59"/>
-      <c r="V88" s="59"/>
+      <c r="K88" s="91"/>
+      <c r="L88" s="91"/>
+      <c r="M88" s="91"/>
+      <c r="N88" s="91"/>
+      <c r="O88" s="91"/>
+      <c r="P88" s="91"/>
+      <c r="Q88" s="91"/>
+      <c r="R88" s="91"/>
+      <c r="S88" s="91"/>
+      <c r="T88" s="91"/>
+      <c r="U88" s="91"/>
+      <c r="V88" s="91"/>
     </row>
     <row r="89" spans="2:32" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="48">
@@ -3262,17 +3265,17 @@
       <c r="E89" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F89" s="84"/>
-      <c r="G89" s="85"/>
-      <c r="H89" s="85"/>
-      <c r="J89" s="59" t="s">
+      <c r="F89" s="63"/>
+      <c r="G89" s="64"/>
+      <c r="H89" s="64"/>
+      <c r="J89" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="K89" s="59"/>
-      <c r="L89" s="59"/>
-      <c r="M89" s="59"/>
-      <c r="N89" s="59"/>
-      <c r="O89" s="59"/>
+      <c r="K89" s="91"/>
+      <c r="L89" s="91"/>
+      <c r="M89" s="91"/>
+      <c r="N89" s="91"/>
+      <c r="O89" s="91"/>
     </row>
     <row r="90" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B90" s="48">
@@ -3287,17 +3290,17 @@
       <c r="E90" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F90" s="84"/>
-      <c r="G90" s="85"/>
-      <c r="H90" s="85"/>
-      <c r="J90" s="59" t="s">
+      <c r="F90" s="63"/>
+      <c r="G90" s="64"/>
+      <c r="H90" s="64"/>
+      <c r="J90" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="K90" s="59"/>
-      <c r="L90" s="59"/>
-      <c r="M90" s="59"/>
-      <c r="N90" s="59"/>
-      <c r="O90" s="59"/>
+      <c r="K90" s="91"/>
+      <c r="L90" s="91"/>
+      <c r="M90" s="91"/>
+      <c r="N90" s="91"/>
+      <c r="O90" s="91"/>
     </row>
     <row r="91" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B91" s="48">
@@ -3312,17 +3315,17 @@
       <c r="E91" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F91" s="84"/>
-      <c r="G91" s="85"/>
-      <c r="H91" s="85"/>
-      <c r="J91" s="59" t="s">
+      <c r="F91" s="63"/>
+      <c r="G91" s="64"/>
+      <c r="H91" s="64"/>
+      <c r="J91" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="K91" s="59"/>
-      <c r="L91" s="59"/>
-      <c r="M91" s="59"/>
-      <c r="N91" s="59"/>
-      <c r="O91" s="59"/>
+      <c r="K91" s="91"/>
+      <c r="L91" s="91"/>
+      <c r="M91" s="91"/>
+      <c r="N91" s="91"/>
+      <c r="O91" s="91"/>
     </row>
     <row r="92" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B92" s="57">
@@ -3337,30 +3340,30 @@
       <c r="E92" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F92" s="84"/>
-      <c r="G92" s="85"/>
-      <c r="H92" s="85"/>
-      <c r="J92" s="59" t="s">
+      <c r="F92" s="63"/>
+      <c r="G92" s="64"/>
+      <c r="H92" s="64"/>
+      <c r="J92" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="K92" s="59"/>
-      <c r="L92" s="59"/>
-      <c r="M92" s="59"/>
-      <c r="N92" s="59"/>
-      <c r="O92" s="59"/>
-      <c r="T92" s="59"/>
-      <c r="U92" s="59"/>
-      <c r="V92" s="59"/>
-      <c r="W92" s="59"/>
-      <c r="X92" s="59"/>
-      <c r="Y92" s="59"/>
-      <c r="Z92" s="59"/>
-      <c r="AA92" s="59"/>
-      <c r="AB92" s="59"/>
-      <c r="AC92" s="59"/>
-      <c r="AD92" s="59"/>
-      <c r="AE92" s="59"/>
-      <c r="AF92" s="59"/>
+      <c r="K92" s="91"/>
+      <c r="L92" s="91"/>
+      <c r="M92" s="91"/>
+      <c r="N92" s="91"/>
+      <c r="O92" s="91"/>
+      <c r="T92" s="91"/>
+      <c r="U92" s="91"/>
+      <c r="V92" s="91"/>
+      <c r="W92" s="91"/>
+      <c r="X92" s="91"/>
+      <c r="Y92" s="91"/>
+      <c r="Z92" s="91"/>
+      <c r="AA92" s="91"/>
+      <c r="AB92" s="91"/>
+      <c r="AC92" s="91"/>
+      <c r="AD92" s="91"/>
+      <c r="AE92" s="91"/>
+      <c r="AF92" s="91"/>
     </row>
     <row r="93" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B93" s="48">
@@ -3375,17 +3378,17 @@
       <c r="E93" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F93" s="84"/>
-      <c r="G93" s="85"/>
-      <c r="H93" s="85"/>
-      <c r="J93" s="59" t="s">
+      <c r="F93" s="63"/>
+      <c r="G93" s="64"/>
+      <c r="H93" s="64"/>
+      <c r="J93" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="K93" s="59"/>
-      <c r="L93" s="59"/>
-      <c r="M93" s="59"/>
-      <c r="N93" s="59"/>
-      <c r="O93" s="59"/>
+      <c r="K93" s="91"/>
+      <c r="L93" s="91"/>
+      <c r="M93" s="91"/>
+      <c r="N93" s="91"/>
+      <c r="O93" s="91"/>
     </row>
     <row r="94" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B94" s="48">
@@ -3400,17 +3403,17 @@
       <c r="E94" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F94" s="84"/>
-      <c r="G94" s="85"/>
-      <c r="H94" s="85"/>
-      <c r="J94" s="59" t="s">
+      <c r="F94" s="63"/>
+      <c r="G94" s="64"/>
+      <c r="H94" s="64"/>
+      <c r="J94" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="K94" s="59"/>
-      <c r="L94" s="59"/>
-      <c r="M94" s="59"/>
-      <c r="N94" s="59"/>
-      <c r="O94" s="59"/>
+      <c r="K94" s="91"/>
+      <c r="L94" s="91"/>
+      <c r="M94" s="91"/>
+      <c r="N94" s="91"/>
+      <c r="O94" s="91"/>
     </row>
     <row r="95" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B95" s="48">
@@ -3425,17 +3428,17 @@
       <c r="E95" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F95" s="84"/>
-      <c r="G95" s="85"/>
-      <c r="H95" s="85"/>
-      <c r="J95" s="59" t="s">
+      <c r="F95" s="63"/>
+      <c r="G95" s="64"/>
+      <c r="H95" s="64"/>
+      <c r="J95" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="K95" s="59"/>
-      <c r="L95" s="59"/>
-      <c r="M95" s="59"/>
-      <c r="N95" s="59"/>
-      <c r="O95" s="59"/>
+      <c r="K95" s="91"/>
+      <c r="L95" s="91"/>
+      <c r="M95" s="91"/>
+      <c r="N95" s="91"/>
+      <c r="O95" s="91"/>
     </row>
     <row r="96" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B96" s="48">
@@ -3450,17 +3453,17 @@
       <c r="E96" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F96" s="84"/>
-      <c r="G96" s="85"/>
-      <c r="H96" s="85"/>
-      <c r="J96" s="59" t="s">
+      <c r="F96" s="63"/>
+      <c r="G96" s="64"/>
+      <c r="H96" s="64"/>
+      <c r="J96" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="K96" s="59"/>
-      <c r="L96" s="59"/>
-      <c r="M96" s="59"/>
-      <c r="N96" s="59"/>
-      <c r="O96" s="59"/>
+      <c r="K96" s="91"/>
+      <c r="L96" s="91"/>
+      <c r="M96" s="91"/>
+      <c r="N96" s="91"/>
+      <c r="O96" s="91"/>
     </row>
     <row r="97" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B97" s="48">
@@ -3475,17 +3478,17 @@
       <c r="E97" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F97" s="84"/>
-      <c r="G97" s="85"/>
-      <c r="H97" s="85"/>
-      <c r="J97" s="59" t="s">
+      <c r="F97" s="63"/>
+      <c r="G97" s="64"/>
+      <c r="H97" s="64"/>
+      <c r="J97" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="K97" s="59"/>
-      <c r="L97" s="59"/>
-      <c r="M97" s="59"/>
-      <c r="N97" s="59"/>
-      <c r="O97" s="59"/>
+      <c r="K97" s="91"/>
+      <c r="L97" s="91"/>
+      <c r="M97" s="91"/>
+      <c r="N97" s="91"/>
+      <c r="O97" s="91"/>
     </row>
     <row r="98" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B98" s="48">
@@ -3500,17 +3503,17 @@
       <c r="E98" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F98" s="84"/>
-      <c r="G98" s="85"/>
-      <c r="H98" s="85"/>
-      <c r="J98" s="59" t="s">
+      <c r="F98" s="63"/>
+      <c r="G98" s="64"/>
+      <c r="H98" s="64"/>
+      <c r="J98" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="K98" s="59"/>
-      <c r="L98" s="59"/>
-      <c r="M98" s="59"/>
-      <c r="N98" s="59"/>
-      <c r="O98" s="59"/>
+      <c r="K98" s="91"/>
+      <c r="L98" s="91"/>
+      <c r="M98" s="91"/>
+      <c r="N98" s="91"/>
+      <c r="O98" s="91"/>
     </row>
     <row r="99" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B99" s="48">
@@ -3525,17 +3528,17 @@
       <c r="E99" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F99" s="84"/>
-      <c r="G99" s="85"/>
-      <c r="H99" s="85"/>
-      <c r="J99" s="59" t="s">
+      <c r="F99" s="63"/>
+      <c r="G99" s="64"/>
+      <c r="H99" s="64"/>
+      <c r="J99" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="K99" s="59"/>
-      <c r="L99" s="59"/>
-      <c r="M99" s="59"/>
-      <c r="N99" s="59"/>
-      <c r="O99" s="59"/>
+      <c r="K99" s="91"/>
+      <c r="L99" s="91"/>
+      <c r="M99" s="91"/>
+      <c r="N99" s="91"/>
+      <c r="O99" s="91"/>
     </row>
     <row r="100" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B100" s="48">
@@ -3550,17 +3553,17 @@
       <c r="E100" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F100" s="84"/>
-      <c r="G100" s="85"/>
-      <c r="H100" s="85"/>
-      <c r="J100" s="59" t="s">
+      <c r="F100" s="63"/>
+      <c r="G100" s="64"/>
+      <c r="H100" s="64"/>
+      <c r="J100" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="K100" s="59"/>
-      <c r="L100" s="59"/>
-      <c r="M100" s="59"/>
-      <c r="N100" s="59"/>
-      <c r="O100" s="59"/>
+      <c r="K100" s="91"/>
+      <c r="L100" s="91"/>
+      <c r="M100" s="91"/>
+      <c r="N100" s="91"/>
+      <c r="O100" s="91"/>
     </row>
     <row r="101" spans="2:23" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" s="48">
@@ -3575,9 +3578,9 @@
       <c r="E101" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F101" s="84"/>
-      <c r="G101" s="85"/>
-      <c r="H101" s="85"/>
+      <c r="F101" s="63"/>
+      <c r="G101" s="64"/>
+      <c r="H101" s="64"/>
       <c r="J101" s="28" t="s">
         <v>65</v>
       </c>
@@ -3600,9 +3603,9 @@
       <c r="E102" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F102" s="84"/>
-      <c r="G102" s="85"/>
-      <c r="H102" s="85"/>
+      <c r="F102" s="63"/>
+      <c r="G102" s="64"/>
+      <c r="H102" s="64"/>
       <c r="J102" s="28" t="s">
         <v>64</v>
       </c>
@@ -3633,9 +3636,9 @@
       <c r="E103" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F103" s="84"/>
-      <c r="G103" s="85"/>
-      <c r="H103" s="85"/>
+      <c r="F103" s="63"/>
+      <c r="G103" s="64"/>
+      <c r="H103" s="64"/>
       <c r="J103" s="28" t="s">
         <v>66</v>
       </c>
@@ -3658,9 +3661,9 @@
       <c r="E104" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F104" s="84"/>
-      <c r="G104" s="85"/>
-      <c r="H104" s="85"/>
+      <c r="F104" s="63"/>
+      <c r="G104" s="64"/>
+      <c r="H104" s="64"/>
       <c r="J104" s="28" t="s">
         <v>67</v>
       </c>
@@ -3678,9 +3681,9 @@
       <c r="E105" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F105" s="84"/>
-      <c r="G105" s="85"/>
-      <c r="H105" s="85"/>
+      <c r="F105" s="63"/>
+      <c r="G105" s="64"/>
+      <c r="H105" s="64"/>
       <c r="J105" s="28" t="s">
         <v>68</v>
       </c>
@@ -3698,9 +3701,9 @@
       <c r="E106" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F106" s="84"/>
-      <c r="G106" s="85"/>
-      <c r="H106" s="85"/>
+      <c r="F106" s="63"/>
+      <c r="G106" s="64"/>
+      <c r="H106" s="64"/>
       <c r="J106" s="28" t="s">
         <v>69</v>
       </c>
@@ -3718,9 +3721,9 @@
       <c r="E107" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F107" s="84"/>
-      <c r="G107" s="85"/>
-      <c r="H107" s="85"/>
+      <c r="F107" s="63"/>
+      <c r="G107" s="64"/>
+      <c r="H107" s="64"/>
       <c r="J107" s="28" t="s">
         <v>70</v>
       </c>
@@ -3738,9 +3741,9 @@
       <c r="E108" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F108" s="84"/>
-      <c r="G108" s="85"/>
-      <c r="H108" s="85"/>
+      <c r="F108" s="63"/>
+      <c r="G108" s="64"/>
+      <c r="H108" s="64"/>
       <c r="J108" s="28" t="s">
         <v>71</v>
       </c>
@@ -3758,9 +3761,9 @@
       <c r="E109" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F109" s="84"/>
-      <c r="G109" s="85"/>
-      <c r="H109" s="85"/>
+      <c r="F109" s="63"/>
+      <c r="G109" s="64"/>
+      <c r="H109" s="64"/>
       <c r="J109" s="28" t="s">
         <v>72</v>
       </c>
@@ -3778,9 +3781,9 @@
       <c r="E110" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F110" s="84"/>
-      <c r="G110" s="85"/>
-      <c r="H110" s="85"/>
+      <c r="F110" s="63"/>
+      <c r="G110" s="64"/>
+      <c r="H110" s="64"/>
       <c r="J110" s="28" t="s">
         <v>73</v>
       </c>
@@ -3798,9 +3801,9 @@
       <c r="E111" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F111" s="84"/>
-      <c r="G111" s="85"/>
-      <c r="H111" s="85"/>
+      <c r="F111" s="63"/>
+      <c r="G111" s="64"/>
+      <c r="H111" s="64"/>
       <c r="J111" s="28" t="s">
         <v>74</v>
       </c>
@@ -3818,9 +3821,9 @@
       <c r="E112" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F112" s="84"/>
-      <c r="G112" s="85"/>
-      <c r="H112" s="85"/>
+      <c r="F112" s="63"/>
+      <c r="G112" s="64"/>
+      <c r="H112" s="64"/>
       <c r="J112" s="28" t="s">
         <v>47</v>
       </c>
@@ -3838,9 +3841,9 @@
       <c r="E113" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F113" s="86"/>
-      <c r="G113" s="87"/>
-      <c r="H113" s="87"/>
+      <c r="F113" s="65"/>
+      <c r="G113" s="66"/>
+      <c r="H113" s="66"/>
       <c r="J113" s="28" t="s">
         <v>75</v>
       </c>
@@ -3858,9 +3861,9 @@
       <c r="E114" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F114" s="86"/>
-      <c r="G114" s="87"/>
-      <c r="H114" s="87"/>
+      <c r="F114" s="65"/>
+      <c r="G114" s="66"/>
+      <c r="H114" s="66"/>
       <c r="J114" s="28" t="s">
         <v>76</v>
       </c>
@@ -3878,9 +3881,9 @@
       <c r="E115" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F115" s="86"/>
-      <c r="G115" s="87"/>
-      <c r="H115" s="87"/>
+      <c r="F115" s="65"/>
+      <c r="G115" s="66"/>
+      <c r="H115" s="66"/>
       <c r="J115" s="28" t="s">
         <v>77</v>
       </c>
@@ -3898,9 +3901,9 @@
       <c r="E116" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F116" s="84"/>
-      <c r="G116" s="85"/>
-      <c r="H116" s="85"/>
+      <c r="F116" s="63"/>
+      <c r="G116" s="64"/>
+      <c r="H116" s="64"/>
       <c r="J116" s="28" t="s">
         <v>78</v>
       </c>
@@ -3918,9 +3921,9 @@
       <c r="E117" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F117" s="84"/>
-      <c r="G117" s="85"/>
-      <c r="H117" s="85"/>
+      <c r="F117" s="63"/>
+      <c r="G117" s="64"/>
+      <c r="H117" s="64"/>
       <c r="J117" s="28" t="s">
         <v>79</v>
       </c>
@@ -3938,9 +3941,9 @@
       <c r="E118" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F118" s="84"/>
-      <c r="G118" s="85"/>
-      <c r="H118" s="85"/>
+      <c r="F118" s="63"/>
+      <c r="G118" s="64"/>
+      <c r="H118" s="64"/>
       <c r="J118" s="28" t="s">
         <v>80</v>
       </c>
@@ -3958,9 +3961,9 @@
       <c r="E119" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F119" s="84"/>
-      <c r="G119" s="85"/>
-      <c r="H119" s="85"/>
+      <c r="F119" s="63"/>
+      <c r="G119" s="64"/>
+      <c r="H119" s="64"/>
       <c r="J119" s="28" t="s">
         <v>109</v>
       </c>
@@ -3978,9 +3981,9 @@
       <c r="E120" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F120" s="84"/>
-      <c r="G120" s="85"/>
-      <c r="H120" s="85"/>
+      <c r="F120" s="63"/>
+      <c r="G120" s="64"/>
+      <c r="H120" s="64"/>
       <c r="J120" s="28" t="s">
         <v>110</v>
       </c>
@@ -3998,9 +4001,9 @@
       <c r="E121" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F121" s="84"/>
-      <c r="G121" s="85"/>
-      <c r="H121" s="85"/>
+      <c r="F121" s="63"/>
+      <c r="G121" s="64"/>
+      <c r="H121" s="64"/>
       <c r="J121" s="28" t="s">
         <v>111</v>
       </c>
@@ -4016,11 +4019,11 @@
         <v>24</v>
       </c>
       <c r="E122" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F122" s="86"/>
-      <c r="G122" s="87"/>
-      <c r="H122" s="87"/>
+        <v>34</v>
+      </c>
+      <c r="F122" s="65"/>
+      <c r="G122" s="66"/>
+      <c r="H122" s="66"/>
       <c r="J122" s="28" t="s">
         <v>112</v>
       </c>
@@ -4036,11 +4039,13 @@
         <v>24</v>
       </c>
       <c r="E123" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F123" s="86"/>
-      <c r="G123" s="87"/>
-      <c r="H123" s="87"/>
+        <v>34</v>
+      </c>
+      <c r="F123" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="G123" s="66"/>
+      <c r="H123" s="66"/>
       <c r="J123" s="28" t="s">
         <v>113</v>
       </c>
@@ -4056,11 +4061,13 @@
         <v>24</v>
       </c>
       <c r="E124" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F124" s="86"/>
-      <c r="G124" s="87"/>
-      <c r="H124" s="87"/>
+        <v>34</v>
+      </c>
+      <c r="F124" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="G124" s="66"/>
+      <c r="H124" s="66"/>
       <c r="J124" s="28" t="s">
         <v>114</v>
       </c>
@@ -4078,9 +4085,9 @@
       <c r="E125" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F125" s="86"/>
-      <c r="G125" s="87"/>
-      <c r="H125" s="87"/>
+      <c r="F125" s="65"/>
+      <c r="G125" s="66"/>
+      <c r="H125" s="66"/>
       <c r="J125" s="28" t="s">
         <v>115</v>
       </c>
@@ -4098,9 +4105,9 @@
       <c r="E126" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F126" s="86"/>
-      <c r="G126" s="87"/>
-      <c r="H126" s="87"/>
+      <c r="F126" s="65"/>
+      <c r="G126" s="66"/>
+      <c r="H126" s="66"/>
       <c r="J126" s="28" t="s">
         <v>116</v>
       </c>
@@ -4118,9 +4125,9 @@
       <c r="E127" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="F127" s="88"/>
-      <c r="G127" s="89"/>
-      <c r="H127" s="89"/>
+      <c r="F127" s="59"/>
+      <c r="G127" s="60"/>
+      <c r="H127" s="60"/>
       <c r="J127" s="44"/>
       <c r="K127" s="39"/>
       <c r="L127" s="39"/>
@@ -4147,9 +4154,9 @@
       <c r="E128" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F128" s="90"/>
-      <c r="G128" s="91"/>
-      <c r="H128" s="91"/>
+      <c r="F128" s="61"/>
+      <c r="G128" s="62"/>
+      <c r="H128" s="62"/>
       <c r="J128" s="45"/>
       <c r="K128" s="39"/>
       <c r="L128" s="39"/>
@@ -4176,9 +4183,9 @@
       <c r="E129" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F129" s="90"/>
-      <c r="G129" s="91"/>
-      <c r="H129" s="91"/>
+      <c r="F129" s="61"/>
+      <c r="G129" s="62"/>
+      <c r="H129" s="62"/>
       <c r="J129" s="45"/>
       <c r="K129" s="39"/>
       <c r="L129" s="39"/>
@@ -4205,9 +4212,9 @@
       <c r="E130" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F130" s="90"/>
-      <c r="G130" s="91"/>
-      <c r="H130" s="91"/>
+      <c r="F130" s="61"/>
+      <c r="G130" s="62"/>
+      <c r="H130" s="62"/>
       <c r="J130" s="45"/>
       <c r="K130" s="39"/>
       <c r="L130" s="39"/>
@@ -4234,9 +4241,9 @@
       <c r="E131" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F131" s="90"/>
-      <c r="G131" s="91"/>
-      <c r="H131" s="91"/>
+      <c r="F131" s="61"/>
+      <c r="G131" s="62"/>
+      <c r="H131" s="62"/>
       <c r="J131" s="45"/>
       <c r="K131" s="39"/>
       <c r="L131" s="39"/>
@@ -4263,9 +4270,9 @@
       <c r="E132" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F132" s="90"/>
-      <c r="G132" s="91"/>
-      <c r="H132" s="91"/>
+      <c r="F132" s="61"/>
+      <c r="G132" s="62"/>
+      <c r="H132" s="62"/>
       <c r="J132" s="45"/>
       <c r="K132" s="39"/>
       <c r="L132" s="39"/>
@@ -4292,9 +4299,9 @@
       <c r="E133" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F133" s="90"/>
-      <c r="G133" s="91"/>
-      <c r="H133" s="91"/>
+      <c r="F133" s="61"/>
+      <c r="G133" s="62"/>
+      <c r="H133" s="62"/>
       <c r="J133" s="45"/>
       <c r="K133" s="39"/>
       <c r="L133" s="39"/>
@@ -4313,53 +4320,48 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="wIw7k+zan7qvtpME94yAexRzLQm6Z+r+q/36WNJCEZxKYdbB1uEkjY2RWJyWcQWfqj4gAYVRkN2IL0ebuCpNcg==" saltValue="NgYup0/meV0WGTaqa+djGQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="113">
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="F126:H126"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="F130:H130"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="J87:V87"/>
+    <mergeCell ref="J88:V88"/>
+    <mergeCell ref="T92:AF92"/>
+    <mergeCell ref="J100:O100"/>
+    <mergeCell ref="J95:O95"/>
+    <mergeCell ref="J96:O96"/>
+    <mergeCell ref="J97:O97"/>
+    <mergeCell ref="J98:O98"/>
+    <mergeCell ref="J99:O99"/>
+    <mergeCell ref="J91:O91"/>
+    <mergeCell ref="J92:O92"/>
+    <mergeCell ref="J93:O93"/>
+    <mergeCell ref="J94:O94"/>
+    <mergeCell ref="J89:O89"/>
+    <mergeCell ref="J90:O90"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="C81:G81"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="C61:G61"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="C76:G76"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:H3"/>
@@ -4384,48 +4386,53 @@
     <mergeCell ref="C69:G69"/>
     <mergeCell ref="C55:G55"/>
     <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C80:G80"/>
-    <mergeCell ref="C81:G81"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="C61:G61"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="C75:G75"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="J87:V87"/>
-    <mergeCell ref="J88:V88"/>
-    <mergeCell ref="T92:AF92"/>
-    <mergeCell ref="J100:O100"/>
-    <mergeCell ref="J95:O95"/>
-    <mergeCell ref="J96:O96"/>
-    <mergeCell ref="J97:O97"/>
-    <mergeCell ref="J98:O98"/>
-    <mergeCell ref="J99:O99"/>
-    <mergeCell ref="J91:O91"/>
-    <mergeCell ref="J92:O92"/>
-    <mergeCell ref="J93:O93"/>
-    <mergeCell ref="J94:O94"/>
-    <mergeCell ref="J89:O89"/>
-    <mergeCell ref="J90:O90"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="F132:H132"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>